<commit_message>
changed 2.xlsx and added to commit
</commit_message>
<xml_diff>
--- a/2.xlsx
+++ b/2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vipul\Desktop\git_tutorial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA066861-2D5C-4CF2-936F-FF25962B3FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF61B09-1E05-4DBC-A65D-17F51D63E8FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4560" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,9 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>c</t>
+  </si>
+  <si>
+    <t>bbb</t>
   </si>
 </sst>
 </file>
@@ -345,15 +348,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B9"/>
+  <dimension ref="B8:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>0</v>
       </c>

</xml_diff>